<commit_message>
added extra urls of vi_vn
</commit_message>
<xml_diff>
--- a/docs/Language Waves/wave4.xlsx
+++ b/docs/Language Waves/wave4.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agarnepu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OVW Migration\OVWMigration\docs\Language Waves\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="210" windowWidth="19140" windowHeight="6705" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="210" windowWidth="19140" windowHeight="6705" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="en_vn" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="269">
   <si>
     <t>http://www.cisco.com/web/VN/ordering/index.html</t>
   </si>
@@ -818,6 +818,30 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/PH/products/security/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/VN/solutions_vn/strategy/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/VN/products_vn/routers/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/VN/products_vn/routers/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/VN/products_vn/switches/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/VN/products_vn/switches/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/VN/products_vn/wireless/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/VN/products_vn/wireless/products.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/VN/products_vn/security/products.html</t>
   </si>
 </sst>
 </file>
@@ -1536,14 +1560,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1663,6 +1689,139 @@
         <v>71</v>
       </c>
       <c r="E9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>262</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>263</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>264</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>265</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>266</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>267</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>268</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1686,7 +1845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
wave4.xlsx modification with missed url's
</commit_message>
<xml_diff>
--- a/docs/Language Waves/wave4.xlsx
+++ b/docs/Language Waves/wave4.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="330" windowWidth="19140" windowHeight="6585" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="336" windowWidth="19140" windowHeight="6588" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="en_vn" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">zh_intl!$A$1:$A$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">zh_tw!$A$1:$E$39</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="279">
   <si>
     <t>http://www.cisco.com/web/VN/ordering/index.html</t>
   </si>
@@ -837,6 +837,36 @@
   </si>
   <si>
     <t>http://www.cisco.com/web/PH/solutions/strategy.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/VN/products/services.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/VN/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/VN/solutions_vn/executive/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/VN/products_vn/security/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PH/solutions/executive/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/PH/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/MY/solutions/trends/cloud/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/MY/services/order-services/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ID/products/storage/index.html</t>
+  </si>
+  <si>
+    <t>http://www.cisco.com/web/ID/products/storage/products.html</t>
   </si>
 </sst>
 </file>
@@ -888,12 +918,40 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -906,7 +964,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -915,6 +973,11 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -1222,20 +1285,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD22"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1309,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>84</v>
       </c>
@@ -1260,7 +1323,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>85</v>
       </c>
@@ -1271,7 +1334,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -1282,7 +1345,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1293,7 +1356,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1307,7 +1370,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1324,7 +1387,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -1341,7 +1404,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1355,7 +1418,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>240</v>
       </c>
@@ -1369,7 +1432,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>241</v>
       </c>
@@ -1386,7 +1449,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>242</v>
       </c>
@@ -1403,7 +1466,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>243</v>
       </c>
@@ -1420,7 +1483,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>244</v>
       </c>
@@ -1437,7 +1500,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>245</v>
       </c>
@@ -1454,7 +1517,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>246</v>
       </c>
@@ -1471,7 +1534,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>247</v>
       </c>
@@ -1488,7 +1551,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>248</v>
       </c>
@@ -1505,7 +1568,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>249</v>
       </c>
@@ -1522,7 +1585,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>250</v>
       </c>
@@ -1536,6 +1599,34 @@
         <v>71</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="C22" t="s">
+        <v>116</v>
+      </c>
+      <c r="D22" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1548,6 +1639,8 @@
     <hyperlink ref="A4" r:id="rId5"/>
     <hyperlink ref="A11" r:id="rId6"/>
     <hyperlink ref="A10" r:id="rId7"/>
+    <hyperlink ref="A21" r:id="rId8"/>
+    <hyperlink ref="A22" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1555,16 +1648,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="64.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1817,6 +1910,40 @@
         <v>71</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1832,6 +1959,8 @@
     <hyperlink ref="A8" r:id="rId8"/>
     <hyperlink ref="A9" r:id="rId9"/>
     <hyperlink ref="A15" r:id="rId10"/>
+    <hyperlink ref="A18" r:id="rId11"/>
+    <hyperlink ref="A19" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1839,16 +1968,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2138,11 +2267,44 @@
         <v>176</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C21" t="s">
+        <v>116</v>
+      </c>
+      <c r="D21" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
     <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A20" r:id="rId4"/>
+    <hyperlink ref="A21" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2156,11 +2318,11 @@
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="82" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -2977,11 +3139,11 @@
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="83.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="83.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3795,14 +3957,14 @@
   <dimension ref="A1:E49"/>
   <sheetViews>
     <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="85.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="85.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4605,16 +4767,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD22"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="55.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4887,6 +5049,37 @@
         <v>63</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="B19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="C20" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>176</v>
       </c>
     </row>
@@ -4906,6 +5099,8 @@
     <hyperlink ref="A16" r:id="rId12"/>
     <hyperlink ref="A17" r:id="rId13"/>
     <hyperlink ref="A18" r:id="rId14"/>
+    <hyperlink ref="A19" r:id="rId15"/>
+    <hyperlink ref="A20" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4913,20 +5108,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="82" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>190</v>
       </c>
@@ -4943,7 +5138,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>191</v>
       </c>
@@ -4960,7 +5155,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>192</v>
       </c>
@@ -4977,7 +5172,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>193</v>
       </c>
@@ -4994,7 +5189,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>194</v>
       </c>
@@ -5011,7 +5206,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>195</v>
       </c>
@@ -5028,7 +5223,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>196</v>
       </c>
@@ -5045,7 +5240,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>197</v>
       </c>
@@ -5062,7 +5257,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>198</v>
       </c>
@@ -5076,7 +5271,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>199</v>
       </c>
@@ -5090,7 +5285,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>200</v>
       </c>
@@ -5101,7 +5296,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>201</v>
       </c>
@@ -5115,7 +5310,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>202</v>
       </c>
@@ -5126,7 +5321,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>203</v>
       </c>
@@ -5137,7 +5332,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>204</v>
       </c>
@@ -5154,7 +5349,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>205</v>
       </c>
@@ -5183,7 +5378,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>207</v>
       </c>
@@ -5200,7 +5395,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>208</v>
       </c>
@@ -5214,7 +5409,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>209</v>
       </c>
@@ -5225,7 +5420,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>210</v>
       </c>
@@ -5239,7 +5434,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>211</v>
       </c>
@@ -5256,7 +5451,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>212</v>
       </c>
@@ -5273,7 +5468,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>213</v>
       </c>
@@ -5290,7 +5485,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>214</v>
       </c>
@@ -5307,7 +5502,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>215</v>
       </c>
@@ -5324,7 +5519,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>216</v>
       </c>
@@ -5341,7 +5536,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>217</v>
       </c>
@@ -5358,7 +5553,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>218</v>
       </c>
@@ -5375,7 +5570,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>219</v>
       </c>
@@ -5392,7 +5587,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>220</v>
       </c>
@@ -5409,7 +5604,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>221</v>
       </c>
@@ -5426,7 +5621,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>222</v>
       </c>
@@ -5443,7 +5638,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>223</v>
       </c>
@@ -5460,7 +5655,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>224</v>
       </c>
@@ -5477,7 +5672,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>225</v>
       </c>
@@ -5494,7 +5689,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>226</v>
       </c>
@@ -5511,7 +5706,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>227</v>
       </c>
@@ -5528,7 +5723,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>228</v>
       </c>
@@ -5545,7 +5740,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>238</v>
       </c>
@@ -5562,7 +5757,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>239</v>
       </c>
@@ -5576,6 +5771,40 @@
         <v>71</v>
       </c>
       <c r="E41" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" t="s">
+        <v>71</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" s="1" t="s">
         <v>176</v>
       </c>
     </row>
@@ -5611,6 +5840,8 @@
     <hyperlink ref="A28" r:id="rId28"/>
     <hyperlink ref="A29" r:id="rId29"/>
     <hyperlink ref="A30" r:id="rId30"/>
+    <hyperlink ref="A42" r:id="rId31"/>
+    <hyperlink ref="A43" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>